<commit_message>
massive refactoring: text drivers - ph1: jump table
</commit_message>
<xml_diff>
--- a/docs/development/charcode-handlers.xlsx
+++ b/docs/development/charcode-handlers.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20985" windowHeight="10980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20985" windowHeight="10980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="144">
   <si>
     <t>code byte</t>
     <phoneticPr fontId="1"/>
@@ -487,12 +488,3183 @@
 use caller-supplied value as pointer to string</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>$3c:8b78
+$3c:8998</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">param: FF = next exp
+param: 30-FE(inclusive) : $8998(param)
+or param == 00 (status): $8998(0x3e)
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jmp textd.draw_embedded_text (0x00 == param &amp;&amp; (0 != (status &amp; 0xFE)))
+jmp textd.deref_text_id (0x01 == param || 0x02 &lt; param &lt; 0x08)
+jmp textd.draw_in_box (0x02 == param || param &gt;= 0x30)
+jmp textd.deref_param_text_unsafe (0x08 &lt;= param &lt; 0x30)
+jmp textd.continue_with_text (0xFF == param)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>textd_x.ctrl_code_handlers.high_and_flags</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_01) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_02) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_02) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_03) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_04) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_05) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_06) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_07) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_07) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_08) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_09) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0a) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0b) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0d) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0e) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0f) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_10) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_11) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_12) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_13) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_14) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_15) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_16) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_17) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_18) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_18) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_19) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_1a) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1a) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_1b) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1b) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1c) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1d) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1e) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_1f) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_20) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_20) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_21) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.CONTINUE_WITH_TEXT)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_22) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_22) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_23) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_24) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_25) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_26) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_27) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFAAAAAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;.db ((HIGH(textd_x.on_code_0c) - HIGH(textd_x.code_handlers_base)) &amp; $07) | ((textd_x.JUST_CONTINUE)&lt;&lt;4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    .db ((HIGH(textd_x.on_code_0c) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> HIGH(textd_x.code_handlers_base)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFAB6526"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4B83CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ((textd_x.HANDLE_EXIT_IN_OWN)&lt;&lt;4)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +3713,25 @@
     <font>
       <sz val="9"/>
       <color rgb="FFC00000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFAB6526"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4B83CD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFAAAAAA"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -634,6 +3825,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>685800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="57150"/>
+          <a:ext cx="4705350" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Note:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>$eefa</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>は</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>A, X, Y </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>について何の仮定ももっていない</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>(input parameters</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ではない</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,9 +4193,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
@@ -917,799 +4213,809 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="str">
-        <f>DEC2HEX(A2,2)</f>
+      <c r="B3" s="2" t="str">
+        <f>DEC2HEX(A3,2)</f>
         <v>00</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B42" si="0">DEC2HEX(A3,2)</f>
-        <v>01</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f t="shared" ref="B4:B43" si="0">DEC2HEX(A4,2)</f>
+        <v>01</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>02</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>03</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="1">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>04</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>05</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="str">
+      <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>06</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>07</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>08</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>09</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="str">
+      <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0A</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="1">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0B</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="1">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0C</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="1">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0D</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="str">
+      <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0E</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="str">
+      <c r="B18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0F</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="str">
+      <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
+      <c r="G19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="1">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="str">
+      <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21" s="1">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="str">
+      <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="str">
+      <c r="B23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" s="1">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="str">
+      <c r="B24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24" s="1">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="str">
+      <c r="B25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="1">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="str">
+      <c r="B26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="1">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="str">
+      <c r="B27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A27" s="1">
+    <row r="28" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="str">
+      <c r="B28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A28" s="1">
+    <row r="29" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="str">
+      <c r="B29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A29" s="1">
+    <row r="30" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="str">
+      <c r="B30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A30" s="1">
+    <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="str">
+      <c r="B31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A31" s="1">
+    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="str">
+      <c r="B32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="24" x14ac:dyDescent="0.15">
-      <c r="A32" s="1">
+    <row r="33" spans="1:9" ht="24" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="str">
+      <c r="B33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A33" s="1">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="str">
+      <c r="B34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G34" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A34" s="1">
+    <row r="35" spans="1:9" ht="24" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="str">
+      <c r="B35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A35" s="1">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="str">
+      <c r="B36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="24" x14ac:dyDescent="0.15">
-      <c r="A36" s="1">
+    <row r="37" spans="1:9" ht="24" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="2" t="str">
+      <c r="B37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" s="1">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="str">
+      <c r="B38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A38" s="1">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="2" t="str">
+      <c r="B39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A39" s="1">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="str">
+      <c r="B40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A40" s="1">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="2" t="str">
+      <c r="B41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A41" s="1">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="2" t="str">
+      <c r="B42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A42" s="1">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="2" t="str">
+      <c r="B43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -1718,5 +5024,267 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A24" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A25" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A33" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A34" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A35" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A39" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A40" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A41" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A42" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A44" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A48" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>